<commit_message>
clean up some DTO's and configure MovieDTO
</commit_message>
<xml_diff>
--- a/Mediathek/src/main/resources/csv/Movie.xlsx
+++ b/Mediathek/src/main/resources/csv/Movie.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Schule\DBI\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philip\Documents\Schule\DBI\DBIJPA4Mediathek\Mediathek\src\main\resources\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1B4489-7784-494F-84CC-14C2A6C43C03}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -355,11 +356,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,44 +368,89 @@
     <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>